<commit_message>
update fxml area administrativo
</commit_message>
<xml_diff>
--- a/Daily Scrum 3oSprint.xlsx
+++ b/Daily Scrum 3oSprint.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\OneDrive\Ambiente de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\GitHub\upskill_java1_labprg_grupo3\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D1D3BD-2EDF-4C01-AEE5-D5C4F9376FF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12540"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
   <si>
     <t>1- Whats
  been done</t>
@@ -71,12 +72,35 @@
   <si>
     <t>atualizacao da documentacao de analise do uc9
 implementacao das classes de dominio</t>
+  </si>
+  <si>
+    <t>UC2 - PLSQL</t>
+  </si>
+  <si>
+    <t>UC4, UC6 - PLSQL</t>
+  </si>
+  <si>
+    <t>UC1, UC3 - PLSQL
+UC1 - Ligação Modelo com base de dados</t>
+  </si>
+  <si>
+    <t>UC5 - PLSQL
+Inserts Gerais</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Implementação Novas Classes TDD</t>
+  </si>
+  <si>
+    <t>Implementação Novas Classes TDD</t>
+  </si>
+  <si>
+    <t>Finalização PLSQL + ligação modelo com base de dados</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -474,11 +498,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,6 +580,76 @@
         <v>8</v>
       </c>
     </row>
+    <row r="7" spans="1:4" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>44244</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>